<commit_message>
Update daily predictions metrics CSV for improved data accuracy
</commit_message>
<xml_diff>
--- a/daily_predictions_metrics.xlsx
+++ b/daily_predictions_metrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edene\OneDrive\שולחן העבודה\פרויקט גמר\פרויקט גמר\Data\final_data_file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{399A31E0-D667-4E55-88C9-9827FCB202FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5FC257-CB87-434F-9577-FD5E30F287C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -407,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -516,853 +516,1612 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>45821</v>
+        <v>45809</v>
       </c>
       <c r="B5">
-        <v>33.328983000000001</v>
+        <v>32.874546000000002</v>
       </c>
       <c r="C5">
-        <v>20.947441000000001</v>
+        <v>21.74239</v>
       </c>
       <c r="D5">
-        <v>27.512959347222221</v>
+        <v>27.358384763888889</v>
       </c>
       <c r="E5">
-        <v>87.472570000000005</v>
+        <v>89.532660000000007</v>
       </c>
       <c r="F5">
-        <v>58.861384999999999</v>
+        <v>56.237811999999998</v>
       </c>
       <c r="G5">
-        <v>73.67116324305556</v>
+        <v>71.331135930555561</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>45822</v>
+        <v>45810</v>
       </c>
       <c r="B6">
-        <v>33.543624999999999</v>
+        <v>32.844867999999998</v>
       </c>
       <c r="C6">
-        <v>21.698969999999999</v>
+        <v>21.780833999999999</v>
       </c>
       <c r="D6">
-        <v>27.858529854166669</v>
+        <v>27.601145881944451</v>
       </c>
       <c r="E6">
-        <v>88.745239999999995</v>
+        <v>87.466149999999999</v>
       </c>
       <c r="F6">
-        <v>58.445076</v>
+        <v>52.559691999999998</v>
       </c>
       <c r="G6">
-        <v>74.672764548611113</v>
+        <v>70.085212708333344</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>45823</v>
+        <v>45811</v>
       </c>
       <c r="B7">
-        <v>33.192749999999997</v>
+        <v>32.817146000000001</v>
       </c>
       <c r="C7">
-        <v>21.530110000000001</v>
+        <v>21.466866</v>
       </c>
       <c r="D7">
-        <v>27.58002606944444</v>
+        <v>26.88942185416667</v>
       </c>
       <c r="E7">
-        <v>88.348404000000002</v>
+        <v>88.938770000000005</v>
       </c>
       <c r="F7">
-        <v>58.450974000000002</v>
+        <v>55.927906</v>
       </c>
       <c r="G7">
-        <v>74.595050749999999</v>
+        <v>73.916188888888883</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>45824</v>
+        <v>45812</v>
       </c>
       <c r="B8">
-        <v>33.217469999999999</v>
+        <v>32.849460000000001</v>
       </c>
       <c r="C8">
-        <v>22.111940000000001</v>
+        <v>21.875843</v>
       </c>
       <c r="D8">
-        <v>27.67483124475525</v>
+        <v>27.73548239583333</v>
       </c>
       <c r="E8">
-        <v>85.814803999999995</v>
+        <v>85.561109999999999</v>
       </c>
       <c r="F8">
-        <v>54.3765</v>
+        <v>57.54918</v>
       </c>
       <c r="G8">
-        <v>72.567028580419574</v>
+        <v>71.070505006944444</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>45825</v>
+        <v>45813</v>
       </c>
       <c r="B9">
-        <v>33.171059999999997</v>
+        <v>33.604247999999998</v>
       </c>
       <c r="C9">
-        <v>21.362570000000002</v>
+        <v>22.039463000000001</v>
       </c>
       <c r="D9">
-        <v>27.605651111111111</v>
+        <v>27.781657729166671</v>
       </c>
       <c r="E9">
-        <v>89.655395999999996</v>
+        <v>88.243269999999995</v>
       </c>
       <c r="F9">
-        <v>52.281723</v>
+        <v>53.739437000000002</v>
       </c>
       <c r="G9">
-        <v>70.652846562500002</v>
+        <v>71.897193527777787</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>45826</v>
+        <v>45814</v>
       </c>
       <c r="B10">
-        <v>33.553013</v>
+        <v>33.35454</v>
       </c>
       <c r="C10">
-        <v>21.113759999999999</v>
+        <v>21.573502000000001</v>
       </c>
       <c r="D10">
-        <v>27.564531493055551</v>
+        <v>27.623971770833339</v>
       </c>
       <c r="E10">
-        <v>87.391319999999993</v>
+        <v>85.970100000000002</v>
       </c>
       <c r="F10">
-        <v>55.989559999999997</v>
+        <v>57.798476999999998</v>
       </c>
       <c r="G10">
-        <v>72.468705131944432</v>
+        <v>72.928780965277781</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>45827</v>
+        <v>45815</v>
       </c>
       <c r="B11">
-        <v>33.708820000000003</v>
+        <v>33.111255999999997</v>
       </c>
       <c r="C11">
-        <v>20.946954999999999</v>
+        <v>20.379086000000001</v>
       </c>
       <c r="D11">
-        <v>27.658652701388888</v>
+        <v>26.90155418055555</v>
       </c>
       <c r="E11">
-        <v>87.476776000000001</v>
+        <v>98.532814000000002</v>
       </c>
       <c r="F11">
-        <v>58.766753999999999</v>
+        <v>58.251292999999997</v>
       </c>
       <c r="G11">
-        <v>71.865919284722224</v>
+        <v>73.486214423611102</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>45828</v>
+        <v>45816</v>
       </c>
       <c r="B12">
-        <v>33.523940000000003</v>
+        <v>33.378340000000001</v>
       </c>
       <c r="C12">
-        <v>21.473604000000002</v>
+        <v>20.458469999999998</v>
       </c>
       <c r="D12">
-        <v>27.444159423611111</v>
+        <v>27.483862319444441</v>
       </c>
       <c r="E12">
-        <v>92.954440000000005</v>
+        <v>98.959500000000006</v>
       </c>
       <c r="F12">
-        <v>58.215366000000003</v>
+        <v>60.924576000000002</v>
       </c>
       <c r="G12">
-        <v>73.920280069444445</v>
+        <v>76.207383263888886</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>45829</v>
+        <v>45817</v>
       </c>
       <c r="B13">
-        <v>33.523910000000001</v>
+        <v>32.857532999999997</v>
       </c>
       <c r="C13">
-        <v>20.577052999999999</v>
+        <v>21.820820000000001</v>
       </c>
       <c r="D13">
-        <v>27.62882034027778</v>
+        <v>27.482590270833331</v>
       </c>
       <c r="E13">
-        <v>92.699209999999994</v>
+        <v>85.472880000000004</v>
       </c>
       <c r="F13">
-        <v>59.859214999999999</v>
+        <v>56.525886999999997</v>
       </c>
       <c r="G13">
-        <v>74.084793694444443</v>
+        <v>73.643135631944446</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>45830</v>
+        <v>45818</v>
       </c>
       <c r="B14">
-        <v>33.181399999999996</v>
+        <v>33.580530000000003</v>
       </c>
       <c r="C14">
-        <v>21.144625000000001</v>
+        <v>22.292137</v>
       </c>
       <c r="D14">
-        <v>27.705559097222221</v>
+        <v>27.7190653125</v>
       </c>
       <c r="E14">
-        <v>87.054209999999998</v>
+        <v>85.820729999999998</v>
       </c>
       <c r="F14">
-        <v>58.034224999999999</v>
+        <v>54.451183</v>
       </c>
       <c r="G14">
-        <v>74.898565708333336</v>
+        <v>70.718443430555553</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>45831</v>
+        <v>45819</v>
       </c>
       <c r="B15">
-        <v>33.663960000000003</v>
+        <v>33.463633999999999</v>
       </c>
       <c r="C15">
-        <v>24.433668000000001</v>
+        <v>21.676615000000002</v>
       </c>
       <c r="D15">
-        <v>28.657821256944441</v>
+        <v>27.750629631944449</v>
       </c>
       <c r="E15">
-        <v>89.573363999999998</v>
+        <v>86.897019999999998</v>
       </c>
       <c r="F15">
-        <v>54.980038</v>
+        <v>58.63053</v>
       </c>
       <c r="G15">
-        <v>73.15036534722222</v>
+        <v>73.208679618055555</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>45832</v>
+        <v>45820</v>
       </c>
       <c r="B16">
-        <v>33.315280000000001</v>
+        <v>33.575386000000002</v>
       </c>
       <c r="C16">
-        <v>23.164099</v>
+        <v>21.289024000000001</v>
       </c>
       <c r="D16">
-        <v>28.370699347222221</v>
+        <v>27.491128340277779</v>
       </c>
       <c r="E16">
-        <v>87.423270000000002</v>
+        <v>87.699479999999994</v>
       </c>
       <c r="F16">
-        <v>57.18685</v>
+        <v>57.392417999999999</v>
       </c>
       <c r="G16">
-        <v>73.303661416666671</v>
+        <v>72.094355777777778</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>45833</v>
+        <v>45821</v>
       </c>
       <c r="B17">
-        <v>33.323433000000001</v>
+        <v>33.328983000000001</v>
       </c>
       <c r="C17">
-        <v>21.995338</v>
+        <v>20.947441000000001</v>
       </c>
       <c r="D17">
-        <v>28.14272304166667</v>
+        <v>27.512959347222221</v>
       </c>
       <c r="E17">
-        <v>89.074979999999996</v>
+        <v>87.472570000000005</v>
       </c>
       <c r="F17">
-        <v>59.128585999999999</v>
+        <v>58.861384999999999</v>
       </c>
       <c r="G17">
-        <v>73.957125319444444</v>
+        <v>73.67116324305556</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>45834</v>
+        <v>45822</v>
       </c>
       <c r="B18">
-        <v>33.894756000000001</v>
+        <v>33.543624999999999</v>
       </c>
       <c r="C18">
-        <v>21.041744000000001</v>
+        <v>21.698969999999999</v>
       </c>
       <c r="D18">
-        <v>27.844545437499999</v>
+        <v>27.858529854166669</v>
       </c>
       <c r="E18">
-        <v>88.579849999999993</v>
+        <v>88.745239999999995</v>
       </c>
       <c r="F18">
-        <v>58.083064999999998</v>
+        <v>58.445076</v>
       </c>
       <c r="G18">
-        <v>72.170624986111108</v>
+        <v>74.672764548611113</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>45835</v>
+        <v>45823</v>
       </c>
       <c r="B19">
-        <v>34.886355999999999</v>
+        <v>33.192749999999997</v>
       </c>
       <c r="C19">
-        <v>21.285876999999999</v>
+        <v>21.530110000000001</v>
       </c>
       <c r="D19">
-        <v>28.12835484027778</v>
+        <v>27.58002606944444</v>
       </c>
       <c r="E19">
-        <v>88.217315999999997</v>
+        <v>88.348404000000002</v>
       </c>
       <c r="F19">
-        <v>52.805050000000001</v>
+        <v>58.450974000000002</v>
       </c>
       <c r="G19">
-        <v>69.363333604166669</v>
+        <v>74.595050749999999</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>45836</v>
+        <v>45824</v>
       </c>
       <c r="B20">
-        <v>35.222290000000001</v>
+        <v>33.217469999999999</v>
       </c>
       <c r="C20">
-        <v>20.596436000000001</v>
+        <v>22.111940000000001</v>
       </c>
       <c r="D20">
-        <v>28.433587673611111</v>
+        <v>27.67483124475525</v>
       </c>
       <c r="E20">
-        <v>100</v>
+        <v>85.814803999999995</v>
       </c>
       <c r="F20">
-        <v>53.074855999999997</v>
+        <v>54.3765</v>
       </c>
       <c r="G20">
-        <v>71.38407903472222</v>
+        <v>72.567028580419574</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>45837</v>
+        <v>45825</v>
       </c>
       <c r="B21">
-        <v>35.250526000000001</v>
+        <v>33.171059999999997</v>
       </c>
       <c r="C21">
-        <v>20.810352000000002</v>
+        <v>21.362570000000002</v>
       </c>
       <c r="D21">
-        <v>28.445775048611111</v>
+        <v>27.605651111111111</v>
       </c>
       <c r="E21">
-        <v>97.456069999999997</v>
+        <v>89.655395999999996</v>
       </c>
       <c r="F21">
-        <v>54.378211999999998</v>
+        <v>52.281723</v>
       </c>
       <c r="G21">
-        <v>70.616747708333321</v>
+        <v>70.652846562500002</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>45838</v>
+        <v>45826</v>
       </c>
       <c r="B22">
-        <v>34.402349999999998</v>
+        <v>33.553013</v>
       </c>
       <c r="C22">
-        <v>23.648260000000001</v>
+        <v>21.113759999999999</v>
       </c>
       <c r="D22">
-        <v>28.619939883211678</v>
+        <v>27.564531493055551</v>
       </c>
       <c r="E22">
-        <v>89.78228</v>
+        <v>87.391319999999993</v>
       </c>
       <c r="F22">
-        <v>55.587615999999997</v>
+        <v>55.989559999999997</v>
       </c>
       <c r="G22">
-        <v>74.093243554744532</v>
+        <v>72.468705131944432</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>45851</v>
+        <v>45827</v>
       </c>
       <c r="B23">
-        <v>34.184710000000003</v>
+        <v>33.708820000000003</v>
       </c>
       <c r="C23">
-        <v>23.451716999999999</v>
+        <v>20.946954999999999</v>
       </c>
       <c r="D23">
-        <v>28.385018305555558</v>
+        <v>27.658652701388888</v>
       </c>
       <c r="E23">
-        <v>86.825460000000007</v>
+        <v>87.476776000000001</v>
       </c>
       <c r="F23">
-        <v>59.552647</v>
+        <v>58.766753999999999</v>
       </c>
       <c r="G23">
-        <v>73.406861465277785</v>
+        <v>71.865919284722224</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>45852</v>
+        <v>45828</v>
       </c>
       <c r="B24">
-        <v>33.995550000000001</v>
+        <v>33.523940000000003</v>
       </c>
       <c r="C24">
-        <v>21.920273000000002</v>
+        <v>21.473604000000002</v>
       </c>
       <c r="D24">
-        <v>28.269410805555559</v>
+        <v>27.444159423611111</v>
       </c>
       <c r="E24">
-        <v>84.849980000000002</v>
+        <v>92.954440000000005</v>
       </c>
       <c r="F24">
-        <v>56.492783000000003</v>
+        <v>58.215366000000003</v>
       </c>
       <c r="G24">
-        <v>71.649946611111119</v>
+        <v>73.920280069444445</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>45853</v>
+        <v>45829</v>
       </c>
       <c r="B25">
-        <v>33.903004000000003</v>
+        <v>33.523910000000001</v>
       </c>
       <c r="C25">
-        <v>23.200804000000002</v>
+        <v>20.577052999999999</v>
       </c>
       <c r="D25">
-        <v>28.584244375000001</v>
+        <v>27.62882034027778</v>
       </c>
       <c r="E25">
-        <v>86.725525000000005</v>
+        <v>92.699209999999994</v>
       </c>
       <c r="F25">
-        <v>55.928449999999998</v>
+        <v>59.859214999999999</v>
       </c>
       <c r="G25">
-        <v>72.045028798611099</v>
+        <v>74.084793694444443</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>45854</v>
+        <v>45830</v>
       </c>
       <c r="B26">
-        <v>34.936596000000002</v>
+        <v>33.181399999999996</v>
       </c>
       <c r="C26">
-        <v>21.414695999999999</v>
+        <v>21.144625000000001</v>
       </c>
       <c r="D26">
-        <v>28.527219627737221</v>
+        <v>27.705559097222221</v>
       </c>
       <c r="E26">
-        <v>85.734695000000002</v>
+        <v>87.054209999999998</v>
       </c>
       <c r="F26">
-        <v>53.518245999999998</v>
+        <v>58.034224999999999</v>
       </c>
       <c r="G26">
-        <v>68.717991678832121</v>
+        <v>74.898565708333336</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>45855</v>
+        <v>45831</v>
       </c>
       <c r="B27">
-        <v>35.781081999999998</v>
+        <v>33.663960000000003</v>
       </c>
       <c r="C27">
-        <v>20.89752</v>
+        <v>24.433668000000001</v>
       </c>
       <c r="D27">
-        <v>29.504750375</v>
+        <v>28.657821256944441</v>
       </c>
       <c r="E27">
-        <v>96.475999999999999</v>
+        <v>89.573363999999998</v>
       </c>
       <c r="F27">
-        <v>50.862560000000002</v>
+        <v>54.980038</v>
       </c>
       <c r="G27">
-        <v>65.891883951388891</v>
+        <v>73.15036534722222</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>45856</v>
+        <v>45832</v>
       </c>
       <c r="B28">
-        <v>35.160843</v>
+        <v>33.315280000000001</v>
       </c>
       <c r="C28">
-        <v>21.701447000000002</v>
+        <v>23.164099</v>
       </c>
       <c r="D28">
-        <v>28.86575506944445</v>
+        <v>28.370699347222221</v>
       </c>
       <c r="E28">
-        <v>89.61506</v>
+        <v>87.423270000000002</v>
       </c>
       <c r="F28">
-        <v>56.281418000000002</v>
+        <v>57.18685</v>
       </c>
       <c r="G28">
-        <v>71.566403277777781</v>
+        <v>73.303661416666671</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>45857</v>
+        <v>45833</v>
       </c>
       <c r="B29">
-        <v>34.334426999999998</v>
+        <v>33.323433000000001</v>
       </c>
       <c r="C29">
-        <v>23.744335</v>
+        <v>21.995338</v>
       </c>
       <c r="D29">
-        <v>28.978664458333331</v>
+        <v>28.14272304166667</v>
       </c>
       <c r="E29">
-        <v>86.187370000000001</v>
+        <v>89.074979999999996</v>
       </c>
       <c r="F29">
-        <v>56.179442999999999</v>
+        <v>59.128585999999999</v>
       </c>
       <c r="G29">
-        <v>71.43962614583333</v>
+        <v>73.957125319444444</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>45858</v>
+        <v>45834</v>
       </c>
       <c r="B30">
-        <v>34.359271999999997</v>
+        <v>33.894756000000001</v>
       </c>
       <c r="C30">
-        <v>24.579287999999998</v>
+        <v>21.041744000000001</v>
       </c>
       <c r="D30">
-        <v>29.208606340277779</v>
+        <v>27.844545437499999</v>
       </c>
       <c r="E30">
-        <v>85.805139999999994</v>
+        <v>88.579849999999993</v>
       </c>
       <c r="F30">
-        <v>54.521152000000001</v>
+        <v>58.083064999999998</v>
       </c>
       <c r="G30">
-        <v>72.866197298611112</v>
+        <v>72.170624986111108</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>45859</v>
+        <v>45835</v>
       </c>
       <c r="B31">
-        <v>34.499980000000001</v>
+        <v>34.886355999999999</v>
       </c>
       <c r="C31">
-        <v>24.304600000000001</v>
+        <v>21.285876999999999</v>
       </c>
       <c r="D31">
-        <v>29.15367197222222</v>
+        <v>28.12835484027778</v>
       </c>
       <c r="E31">
-        <v>87.234375</v>
+        <v>88.217315999999997</v>
       </c>
       <c r="F31">
-        <v>56.97289</v>
+        <v>52.805050000000001</v>
       </c>
       <c r="G31">
-        <v>73.305430659722219</v>
+        <v>69.363333604166669</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>45860</v>
+        <v>45836</v>
       </c>
       <c r="B32">
-        <v>35.403713000000003</v>
+        <v>35.222290000000001</v>
       </c>
       <c r="C32">
-        <v>23.970219</v>
+        <v>20.596436000000001</v>
       </c>
       <c r="D32">
-        <v>29.290561819444449</v>
+        <v>28.433587673611111</v>
       </c>
       <c r="E32">
-        <v>89.596199999999996</v>
+        <v>100</v>
       </c>
       <c r="F32">
-        <v>55.801963999999998</v>
+        <v>53.074855999999997</v>
       </c>
       <c r="G32">
-        <v>72.220465895833343</v>
+        <v>71.38407903472222</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>45861</v>
+        <v>45837</v>
       </c>
       <c r="B33">
-        <v>35.239432999999998</v>
+        <v>35.250526000000001</v>
       </c>
       <c r="C33">
-        <v>23.379162000000001</v>
+        <v>20.810352000000002</v>
       </c>
       <c r="D33">
-        <v>29.453986444444439</v>
+        <v>28.445775048611111</v>
       </c>
       <c r="E33">
-        <v>85.80847</v>
+        <v>97.456069999999997</v>
       </c>
       <c r="F33">
-        <v>59.485016000000002</v>
+        <v>54.378211999999998</v>
       </c>
       <c r="G33">
-        <v>72.253708541666668</v>
+        <v>70.616747708333321</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>45862</v>
+        <v>45838</v>
       </c>
       <c r="B34">
-        <v>34.682810000000003</v>
+        <v>34.402349999999998</v>
       </c>
       <c r="C34">
-        <v>22.751321999999998</v>
+        <v>23.648260000000001</v>
       </c>
       <c r="D34">
-        <v>29.257433701388891</v>
+        <v>28.75473953146853</v>
       </c>
       <c r="E34">
-        <v>85.852059999999994</v>
+        <v>89.78228</v>
       </c>
       <c r="F34">
-        <v>54.387645999999997</v>
+        <v>55.587615999999997</v>
       </c>
       <c r="G34">
-        <v>72.645715444444434</v>
+        <v>73.58497318881119</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>45863</v>
+        <v>45839</v>
       </c>
       <c r="B35">
-        <v>34.236263000000001</v>
+        <v>36.121229999999997</v>
       </c>
       <c r="C35">
-        <v>22.435915000000001</v>
+        <v>21.843239000000001</v>
       </c>
       <c r="D35">
-        <v>28.936709763888889</v>
+        <v>29.478300999999998</v>
       </c>
       <c r="E35">
-        <v>87.97269</v>
+        <v>90.028880000000001</v>
       </c>
       <c r="F35">
-        <v>62.508087000000003</v>
+        <v>45.274062999999998</v>
       </c>
       <c r="G35">
-        <v>74.276412083333341</v>
+        <v>66.116293034722219</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>45864</v>
+        <v>45840</v>
       </c>
       <c r="B36">
-        <v>34.993110000000001</v>
+        <v>35.164786999999997</v>
       </c>
       <c r="C36">
-        <v>24.679189999999998</v>
+        <v>21.624939999999999</v>
       </c>
       <c r="D36">
-        <v>29.895539381944449</v>
+        <v>28.663491791666669</v>
       </c>
       <c r="E36">
-        <v>87.731359999999995</v>
+        <v>85.255210000000005</v>
       </c>
       <c r="F36">
-        <v>59.260544000000003</v>
+        <v>54.452553000000002</v>
       </c>
       <c r="G36">
-        <v>74.709256965277788</v>
+        <v>68.837101958333335</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>45865</v>
+        <v>45841</v>
       </c>
       <c r="B37">
-        <v>34.988219999999998</v>
+        <v>34.096375000000002</v>
       </c>
       <c r="C37">
-        <v>21.847218000000002</v>
+        <v>21.728345999999998</v>
       </c>
       <c r="D37">
-        <v>29.584516597222219</v>
+        <v>28.289495673611111</v>
       </c>
       <c r="E37">
-        <v>87.946719999999999</v>
+        <v>89.824169999999995</v>
       </c>
       <c r="F37">
-        <v>54.578969999999998</v>
+        <v>58.809600000000003</v>
       </c>
       <c r="G37">
-        <v>70.91445359722222</v>
+        <v>72.977488138888887</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>45866</v>
+        <v>45842</v>
       </c>
       <c r="B38">
-        <v>35.622565999999999</v>
+        <v>34.777119999999996</v>
       </c>
       <c r="C38">
-        <v>25.115036</v>
+        <v>22.005065999999999</v>
       </c>
       <c r="D38">
-        <v>29.631642983870972</v>
+        <v>28.22187125</v>
       </c>
       <c r="E38">
-        <v>90.700299999999999</v>
+        <v>88.011634999999998</v>
       </c>
       <c r="F38">
-        <v>52.906930000000003</v>
+        <v>56.242992000000001</v>
       </c>
       <c r="G38">
-        <v>74.856918741935473</v>
+        <v>72.389513249999993</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>45867</v>
+        <v>45843</v>
       </c>
       <c r="B39">
-        <v>35.155045000000001</v>
+        <v>33.946807999999997</v>
       </c>
       <c r="C39">
-        <v>25.333614000000001</v>
+        <v>21.115777999999999</v>
       </c>
       <c r="D39">
-        <v>30.04926556944444</v>
+        <v>27.942748958333329</v>
       </c>
       <c r="E39">
-        <v>88.965299999999999</v>
+        <v>87.705960000000005</v>
       </c>
       <c r="F39">
-        <v>55.540866999999999</v>
+        <v>57.130885999999997</v>
       </c>
       <c r="G39">
-        <v>71.895573965277777</v>
+        <v>72.406639666666663</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>45868</v>
+        <v>45844</v>
       </c>
       <c r="B40">
-        <v>34.582439999999998</v>
+        <v>34.086799999999997</v>
       </c>
       <c r="C40">
-        <v>25.367594</v>
+        <v>21.675477999999998</v>
       </c>
       <c r="D40">
-        <v>29.420989240875912</v>
+        <v>28.235401986111111</v>
       </c>
       <c r="E40">
-        <v>87.341419999999999</v>
+        <v>86.193420000000003</v>
       </c>
       <c r="F40">
-        <v>54.52966</v>
+        <v>57.531219999999998</v>
       </c>
       <c r="G40">
-        <v>71.492611525547446</v>
+        <v>71.831044673611103</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
+        <v>45845</v>
+      </c>
+      <c r="B41">
+        <v>34.209952999999999</v>
+      </c>
+      <c r="C41">
+        <v>22.626101999999999</v>
+      </c>
+      <c r="D41">
+        <v>28.724086472222229</v>
+      </c>
+      <c r="E41">
+        <v>90.213160000000002</v>
+      </c>
+      <c r="F41">
+        <v>58.396389999999997</v>
+      </c>
+      <c r="G41">
+        <v>74.420092465277776</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>45846</v>
+      </c>
+      <c r="B42">
+        <v>33.907352000000003</v>
+      </c>
+      <c r="C42">
+        <v>23.53708</v>
+      </c>
+      <c r="D42">
+        <v>28.66244161111111</v>
+      </c>
+      <c r="E42">
+        <v>86.447295999999994</v>
+      </c>
+      <c r="F42">
+        <v>60.842261999999998</v>
+      </c>
+      <c r="G42">
+        <v>73.914072958333335</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>45847</v>
+      </c>
+      <c r="B43">
+        <v>34.419117</v>
+      </c>
+      <c r="C43">
+        <v>22.045963</v>
+      </c>
+      <c r="D43">
+        <v>28.28199154166667</v>
+      </c>
+      <c r="E43">
+        <v>89.204390000000004</v>
+      </c>
+      <c r="F43">
+        <v>56.592495</v>
+      </c>
+      <c r="G43">
+        <v>73.01309227083334</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>45848</v>
+      </c>
+      <c r="B44">
+        <v>34.375160000000001</v>
+      </c>
+      <c r="C44">
+        <v>21.458932999999998</v>
+      </c>
+      <c r="D44">
+        <v>28.486128999999998</v>
+      </c>
+      <c r="E44">
+        <v>87.277050000000003</v>
+      </c>
+      <c r="F44">
+        <v>53.534750000000003</v>
+      </c>
+      <c r="G44">
+        <v>73.260532270833338</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>45849</v>
+      </c>
+      <c r="B45">
+        <v>34.874473999999999</v>
+      </c>
+      <c r="C45">
+        <v>24.264809</v>
+      </c>
+      <c r="D45">
+        <v>29.216518638888889</v>
+      </c>
+      <c r="E45">
+        <v>90.813064999999995</v>
+      </c>
+      <c r="F45">
+        <v>54.030074999999997</v>
+      </c>
+      <c r="G45">
+        <v>73.145546770833334</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>45850</v>
+      </c>
+      <c r="B46">
+        <v>35.069870000000002</v>
+      </c>
+      <c r="C46">
+        <v>23.140646</v>
+      </c>
+      <c r="D46">
+        <v>28.585750027777781</v>
+      </c>
+      <c r="E46">
+        <v>93.028509999999997</v>
+      </c>
+      <c r="F46">
+        <v>52.285649999999997</v>
+      </c>
+      <c r="G46">
+        <v>73.416520083333324</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>45851</v>
+      </c>
+      <c r="B47">
+        <v>34.184710000000003</v>
+      </c>
+      <c r="C47">
+        <v>23.451716999999999</v>
+      </c>
+      <c r="D47">
+        <v>28.385018305555558</v>
+      </c>
+      <c r="E47">
+        <v>86.825460000000007</v>
+      </c>
+      <c r="F47">
+        <v>59.552647</v>
+      </c>
+      <c r="G47">
+        <v>73.406861465277785</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>45852</v>
+      </c>
+      <c r="B48">
+        <v>33.995550000000001</v>
+      </c>
+      <c r="C48">
+        <v>21.920273000000002</v>
+      </c>
+      <c r="D48">
+        <v>28.269410805555559</v>
+      </c>
+      <c r="E48">
+        <v>84.849980000000002</v>
+      </c>
+      <c r="F48">
+        <v>56.492783000000003</v>
+      </c>
+      <c r="G48">
+        <v>71.649946611111119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>45853</v>
+      </c>
+      <c r="B49">
+        <v>33.903004000000003</v>
+      </c>
+      <c r="C49">
+        <v>23.200804000000002</v>
+      </c>
+      <c r="D49">
+        <v>28.584244375000001</v>
+      </c>
+      <c r="E49">
+        <v>86.725525000000005</v>
+      </c>
+      <c r="F49">
+        <v>55.928449999999998</v>
+      </c>
+      <c r="G49">
+        <v>72.045028798611099</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>45854</v>
+      </c>
+      <c r="B50">
+        <v>34.936596000000002</v>
+      </c>
+      <c r="C50">
+        <v>21.414695999999999</v>
+      </c>
+      <c r="D50">
+        <v>28.765107741258738</v>
+      </c>
+      <c r="E50">
+        <v>85.734695000000002</v>
+      </c>
+      <c r="F50">
+        <v>53.518245999999998</v>
+      </c>
+      <c r="G50">
+        <v>68.228427384615387</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>45855</v>
+      </c>
+      <c r="B51">
+        <v>35.781081999999998</v>
+      </c>
+      <c r="C51">
+        <v>20.89752</v>
+      </c>
+      <c r="D51">
+        <v>29.504750375</v>
+      </c>
+      <c r="E51">
+        <v>96.475999999999999</v>
+      </c>
+      <c r="F51">
+        <v>50.862560000000002</v>
+      </c>
+      <c r="G51">
+        <v>65.891883951388891</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>45856</v>
+      </c>
+      <c r="B52">
+        <v>35.160843</v>
+      </c>
+      <c r="C52">
+        <v>21.701447000000002</v>
+      </c>
+      <c r="D52">
+        <v>28.86575506944445</v>
+      </c>
+      <c r="E52">
+        <v>89.61506</v>
+      </c>
+      <c r="F52">
+        <v>56.281418000000002</v>
+      </c>
+      <c r="G52">
+        <v>71.566403277777781</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>45857</v>
+      </c>
+      <c r="B53">
+        <v>34.334426999999998</v>
+      </c>
+      <c r="C53">
+        <v>23.744335</v>
+      </c>
+      <c r="D53">
+        <v>28.978664458333331</v>
+      </c>
+      <c r="E53">
+        <v>86.187370000000001</v>
+      </c>
+      <c r="F53">
+        <v>56.179442999999999</v>
+      </c>
+      <c r="G53">
+        <v>71.43962614583333</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>45858</v>
+      </c>
+      <c r="B54">
+        <v>34.359271999999997</v>
+      </c>
+      <c r="C54">
+        <v>24.579287999999998</v>
+      </c>
+      <c r="D54">
+        <v>29.208606340277779</v>
+      </c>
+      <c r="E54">
+        <v>85.805139999999994</v>
+      </c>
+      <c r="F54">
+        <v>54.521152000000001</v>
+      </c>
+      <c r="G54">
+        <v>72.866197298611112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>45859</v>
+      </c>
+      <c r="B55">
+        <v>34.499980000000001</v>
+      </c>
+      <c r="C55">
+        <v>24.304600000000001</v>
+      </c>
+      <c r="D55">
+        <v>29.15367197222222</v>
+      </c>
+      <c r="E55">
+        <v>87.234375</v>
+      </c>
+      <c r="F55">
+        <v>56.97289</v>
+      </c>
+      <c r="G55">
+        <v>73.305430659722219</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>45860</v>
+      </c>
+      <c r="B56">
+        <v>35.403713000000003</v>
+      </c>
+      <c r="C56">
+        <v>23.970219</v>
+      </c>
+      <c r="D56">
+        <v>29.290561819444449</v>
+      </c>
+      <c r="E56">
+        <v>89.596199999999996</v>
+      </c>
+      <c r="F56">
+        <v>55.801963999999998</v>
+      </c>
+      <c r="G56">
+        <v>72.220465895833343</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>45861</v>
+      </c>
+      <c r="B57">
+        <v>35.239432999999998</v>
+      </c>
+      <c r="C57">
+        <v>23.379162000000001</v>
+      </c>
+      <c r="D57">
+        <v>29.453986444444439</v>
+      </c>
+      <c r="E57">
+        <v>85.80847</v>
+      </c>
+      <c r="F57">
+        <v>59.485016000000002</v>
+      </c>
+      <c r="G57">
+        <v>72.253708541666668</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>45862</v>
+      </c>
+      <c r="B58">
+        <v>34.682810000000003</v>
+      </c>
+      <c r="C58">
+        <v>22.751321999999998</v>
+      </c>
+      <c r="D58">
+        <v>29.257433701388891</v>
+      </c>
+      <c r="E58">
+        <v>85.852059999999994</v>
+      </c>
+      <c r="F58">
+        <v>54.387645999999997</v>
+      </c>
+      <c r="G58">
+        <v>72.645715444444434</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>45863</v>
+      </c>
+      <c r="B59">
+        <v>34.236263000000001</v>
+      </c>
+      <c r="C59">
+        <v>22.435915000000001</v>
+      </c>
+      <c r="D59">
+        <v>28.936709763888889</v>
+      </c>
+      <c r="E59">
+        <v>87.97269</v>
+      </c>
+      <c r="F59">
+        <v>62.508087000000003</v>
+      </c>
+      <c r="G59">
+        <v>74.276412083333341</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>45864</v>
+      </c>
+      <c r="B60">
+        <v>34.993110000000001</v>
+      </c>
+      <c r="C60">
+        <v>24.679189999999998</v>
+      </c>
+      <c r="D60">
+        <v>29.895539381944449</v>
+      </c>
+      <c r="E60">
+        <v>87.731359999999995</v>
+      </c>
+      <c r="F60">
+        <v>59.260544000000003</v>
+      </c>
+      <c r="G60">
+        <v>74.709256965277788</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>45865</v>
+      </c>
+      <c r="B61">
+        <v>34.988219999999998</v>
+      </c>
+      <c r="C61">
+        <v>21.847218000000002</v>
+      </c>
+      <c r="D61">
+        <v>29.584516597222219</v>
+      </c>
+      <c r="E61">
+        <v>87.946719999999999</v>
+      </c>
+      <c r="F61">
+        <v>54.578969999999998</v>
+      </c>
+      <c r="G61">
+        <v>70.91445359722222</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>45866</v>
+      </c>
+      <c r="B62">
+        <v>35.622565999999999</v>
+      </c>
+      <c r="C62">
+        <v>25.115036</v>
+      </c>
+      <c r="D62">
+        <v>30.087501701388891</v>
+      </c>
+      <c r="E62">
+        <v>90.700299999999999</v>
+      </c>
+      <c r="F62">
+        <v>52.906930000000003</v>
+      </c>
+      <c r="G62">
+        <v>73.448555722222224</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>45867</v>
+      </c>
+      <c r="B63">
+        <v>35.155045000000001</v>
+      </c>
+      <c r="C63">
+        <v>25.333614000000001</v>
+      </c>
+      <c r="D63">
+        <v>30.04926556944444</v>
+      </c>
+      <c r="E63">
+        <v>88.965299999999999</v>
+      </c>
+      <c r="F63">
+        <v>55.540866999999999</v>
+      </c>
+      <c r="G63">
+        <v>71.895573965277777</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>45868</v>
+      </c>
+      <c r="B64">
+        <v>34.582439999999998</v>
+      </c>
+      <c r="C64">
+        <v>25.367594</v>
+      </c>
+      <c r="D64">
+        <v>29.601060993055551</v>
+      </c>
+      <c r="E64">
+        <v>87.341419999999999</v>
+      </c>
+      <c r="F64">
+        <v>54.52966</v>
+      </c>
+      <c r="G64">
+        <v>71.133206930555559</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
         <v>45869</v>
       </c>
-      <c r="B41">
+      <c r="B65">
         <v>34.290289999999999</v>
       </c>
-      <c r="C41">
+      <c r="C65">
         <v>26.271560000000001</v>
       </c>
-      <c r="D41">
+      <c r="D65">
         <v>29.624577272727269</v>
       </c>
-      <c r="E41">
+      <c r="E65">
         <v>81.206924000000001</v>
       </c>
-      <c r="F41">
+      <c r="F65">
         <v>52.044110000000003</v>
       </c>
-      <c r="G41">
+      <c r="G65">
         <v>68.73123416783217</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>45870</v>
+      </c>
+      <c r="B66">
+        <v>34.351771999999997</v>
+      </c>
+      <c r="C66">
+        <v>24.352705</v>
+      </c>
+      <c r="D66">
+        <v>29.231442459854019</v>
+      </c>
+      <c r="E66">
+        <v>83.919135999999995</v>
+      </c>
+      <c r="F66">
+        <v>53.298496</v>
+      </c>
+      <c r="G66">
+        <v>69.689599970802917</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>45871</v>
+      </c>
+      <c r="B67">
+        <v>35.222442999999998</v>
+      </c>
+      <c r="C67">
+        <v>24.338642</v>
+      </c>
+      <c r="D67">
+        <v>29.309462249999999</v>
+      </c>
+      <c r="E67">
+        <v>85.398139999999998</v>
+      </c>
+      <c r="F67">
+        <v>51.445869999999999</v>
+      </c>
+      <c r="G67">
+        <v>70.352825743055561</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>45872</v>
+      </c>
+      <c r="B68">
+        <v>35.084530000000001</v>
+      </c>
+      <c r="C68">
+        <v>23.922436000000001</v>
+      </c>
+      <c r="D68">
+        <v>29.199996520833331</v>
+      </c>
+      <c r="E68">
+        <v>85.599980000000002</v>
+      </c>
+      <c r="F68">
+        <v>53.868214000000002</v>
+      </c>
+      <c r="G68">
+        <v>69.830330881944448</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>45873</v>
+      </c>
+      <c r="B69">
+        <v>34.698270000000001</v>
+      </c>
+      <c r="C69">
+        <v>22.583082000000001</v>
+      </c>
+      <c r="D69">
+        <v>28.445714083333328</v>
+      </c>
+      <c r="E69">
+        <v>85.242689999999996</v>
+      </c>
+      <c r="F69">
+        <v>55.926319999999997</v>
+      </c>
+      <c r="G69">
+        <v>72.248381465277774</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>45874</v>
+      </c>
+      <c r="B70">
+        <v>34.140433999999999</v>
+      </c>
+      <c r="C70">
+        <v>22.423739999999999</v>
+      </c>
+      <c r="D70">
+        <v>28.301107125000001</v>
+      </c>
+      <c r="E70">
+        <v>84.960440000000006</v>
+      </c>
+      <c r="F70">
+        <v>52.676549999999999</v>
+      </c>
+      <c r="G70">
+        <v>71.399014833333325</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>45875</v>
+      </c>
+      <c r="B71">
+        <v>34.221927999999998</v>
+      </c>
+      <c r="C71">
+        <v>23.542466999999998</v>
+      </c>
+      <c r="D71">
+        <v>29.290372250000001</v>
+      </c>
+      <c r="E71">
+        <v>81.395759999999996</v>
+      </c>
+      <c r="F71">
+        <v>54.852238</v>
+      </c>
+      <c r="G71">
+        <v>70.533312388888888</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>45876</v>
+      </c>
+      <c r="B72">
+        <v>34.686546</v>
+      </c>
+      <c r="C72">
+        <v>23.783591999999999</v>
+      </c>
+      <c r="D72">
+        <v>29.013485534722221</v>
+      </c>
+      <c r="E72">
+        <v>87.84939</v>
+      </c>
+      <c r="F72">
+        <v>54.508842000000001</v>
+      </c>
+      <c r="G72">
+        <v>71.262624541666668</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>45877</v>
+      </c>
+      <c r="B73">
+        <v>34.640625</v>
+      </c>
+      <c r="C73">
+        <v>24.224594</v>
+      </c>
+      <c r="D73">
+        <v>29.673497104166671</v>
+      </c>
+      <c r="E73">
+        <v>83.986760000000004</v>
+      </c>
+      <c r="F73">
+        <v>55.515433999999999</v>
+      </c>
+      <c r="G73">
+        <v>71.228839215277787</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>45878</v>
+      </c>
+      <c r="B74">
+        <v>35.956516000000001</v>
+      </c>
+      <c r="C74">
+        <v>27.307680000000001</v>
+      </c>
+      <c r="D74">
+        <v>30.688723402777779</v>
+      </c>
+      <c r="E74">
+        <v>82.859859999999998</v>
+      </c>
+      <c r="F74">
+        <v>57.09019</v>
+      </c>
+      <c r="G74">
+        <v>71.849557333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>